<commit_message>
Restart experiment of 5-fold
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tse/Downloads/openSMILE-2.1.0/mhmc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tse/Downloads/openSMILE-2.1.0/emotion-recognition/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="32740" yWindow="2960" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="39900" yWindow="1860" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -82,9 +82,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="184" formatCode="0.0000%"/>
-    <numFmt numFmtId="185" formatCode="0.0%"/>
-    <numFmt numFmtId="186" formatCode="0.000%"/>
+    <numFmt numFmtId="176" formatCode="0.0000%"/>
+    <numFmt numFmtId="177" formatCode="0.0%"/>
+    <numFmt numFmtId="178" formatCode="0.000%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -148,22 +148,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="184" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="184" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="186" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="185" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -445,7 +443,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -456,198 +454,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="5">
-        <v>0.88461500000000004</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="B3" s="2">
+        <v>0.85046699999999997</v>
+      </c>
+      <c r="C3" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7">
-        <v>0.836538</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.81308400000000003</v>
+      </c>
+      <c r="C4" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="7">
-        <v>0.80769199999999997</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="B5" s="5">
+        <v>0.82242999999999999</v>
+      </c>
+      <c r="C5" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="7">
-        <v>0.81730800000000003</v>
-      </c>
-      <c r="C6" s="6">
+      <c r="B6" s="4">
+        <v>0.77570099999999997</v>
+      </c>
+      <c r="C6" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="8">
-        <v>0.87395</v>
-      </c>
-      <c r="C7" s="6">
+      <c r="B7" s="4">
+        <v>0.85046699999999997</v>
+      </c>
+      <c r="C7" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="4">
         <v>0.78571400000000002</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="4">
         <v>0.68965500000000002</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="4">
         <v>0.76087000000000005</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="4">
         <v>0.82758600000000004</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="4">
         <v>0.63636400000000004</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="4">
         <v>0.82857099999999995</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="7">
         <v>0.996</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="4">
         <v>0.90163899999999997</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="4">
         <v>0.82608700000000002</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="4">
         <v>0.965665</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="4">
         <v>0.64285700000000001</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="4">
         <v>0.70422499999999999</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Restart experiment of 10-fold
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="39900" yWindow="1860" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="38400" yWindow="1860" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.0000%"/>
-    <numFmt numFmtId="177" formatCode="0.0%"/>
     <numFmt numFmtId="178" formatCode="0.000%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
@@ -148,7 +147,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -158,7 +157,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -443,7 +441,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -454,11 +452,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -525,11 +523,11 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -544,10 +542,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="4">
-        <v>0.78571400000000002</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
+        <v>0.73469399999999996</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.99587599999999998</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="27" x14ac:dyDescent="0.3">
@@ -555,7 +553,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="4">
-        <v>0.68965500000000002</v>
+        <v>0.67241399999999996</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -566,7 +564,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="4">
-        <v>0.76087000000000005</v>
+        <v>0.72092999999999996</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -577,7 +575,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="4">
-        <v>0.82758600000000004</v>
+        <v>0.84210499999999999</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -588,7 +586,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="4">
-        <v>0.63636400000000004</v>
+        <v>0.61818200000000001</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -601,8 +599,8 @@
       <c r="B15" s="4">
         <v>0.82857099999999995</v>
       </c>
-      <c r="C15" s="7">
-        <v>0.996</v>
+      <c r="C15" s="4">
+        <v>0.99599199999999999</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="27" x14ac:dyDescent="0.3">
@@ -610,7 +608,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="4">
-        <v>0.90163899999999997</v>
+        <v>0.88524599999999998</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -624,15 +622,15 @@
         <v>0.82608700000000002</v>
       </c>
       <c r="C17" s="4">
-        <v>0.965665</v>
+        <v>0.96774199999999999</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="4">
-        <v>0.64285700000000001</v>
+      <c r="B18" s="3">
+        <v>0.75</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
@@ -642,8 +640,8 @@
       <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="4">
-        <v>0.70422499999999999</v>
+      <c r="B19" s="5">
+        <v>0.71831</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>

</xml_diff>

<commit_message>
Revise the error of confusionMatrix.py
- Correct the for loop of caculating confusion matrix.
- Re-experiment to correct the result files.
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -81,9 +81,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="176" formatCode="0.0000%"/>
-    <numFmt numFmtId="178" formatCode="0.000%"/>
+    <numFmt numFmtId="177" formatCode="0.000%"/>
+    <numFmt numFmtId="178" formatCode="0.0%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -147,19 +148,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -542,10 +544,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="4">
-        <v>0.73469399999999996</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0.99587599999999998</v>
+        <v>0.75510200000000005</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="27" x14ac:dyDescent="0.3">
@@ -553,7 +555,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="4">
-        <v>0.67241399999999996</v>
+        <v>0.68965500000000002</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -563,7 +565,7 @@
       <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="5">
         <v>0.72092999999999996</v>
       </c>
       <c r="C12" s="3">
@@ -586,7 +588,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="4">
-        <v>0.61818200000000001</v>
+        <v>0.63636400000000004</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -599,8 +601,8 @@
       <c r="B15" s="4">
         <v>0.82857099999999995</v>
       </c>
-      <c r="C15" s="4">
-        <v>0.99599199999999999</v>
+      <c r="C15" s="8">
+        <v>0.996</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="27" x14ac:dyDescent="0.3">
@@ -608,7 +610,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="4">
-        <v>0.88524599999999998</v>
+        <v>0.90163899999999997</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -622,15 +624,15 @@
         <v>0.82608700000000002</v>
       </c>
       <c r="C17" s="4">
-        <v>0.96774199999999999</v>
+        <v>0.965665</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="3">
-        <v>0.75</v>
+      <c r="B18" s="4">
+        <v>0.64285700000000001</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
@@ -640,8 +642,8 @@
       <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="5">
-        <v>0.71831</v>
+      <c r="B19" s="4">
+        <v>0.70422499999999999</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>

</xml_diff>

<commit_message>
Update the algorithm of grouping 5-fold
- Make each emotion type file is average in each group.
- Add the confusion output displaying the number of correct and sum.
- Re-experiment of 5-fold.
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="1860" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="7360" yWindow="900" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -158,10 +158,10 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -443,7 +443,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -454,11 +454,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -474,7 +474,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2">
-        <v>0.85046699999999997</v>
+        <v>0.72897199999999995</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -485,7 +485,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="4">
-        <v>0.81308400000000003</v>
+        <v>0.73831800000000003</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -495,8 +495,8 @@
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="5">
-        <v>0.82242999999999999</v>
+      <c r="B5" s="4">
+        <v>0.77570099999999997</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -506,11 +506,11 @@
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="4">
-        <v>0.77570099999999997</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
+      <c r="B6" s="5">
+        <v>0.71028000000000002</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.97663599999999995</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="27" x14ac:dyDescent="0.3">
@@ -518,18 +518,18 @@
         <v>4</v>
       </c>
       <c r="B7" s="4">
-        <v>0.85046699999999997</v>
+        <v>0.76635500000000001</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -601,7 +601,7 @@
       <c r="B15" s="4">
         <v>0.82857099999999995</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>0.996</v>
       </c>
     </row>

</xml_diff>